<commit_message>
change details about dotnet
</commit_message>
<xml_diff>
--- a/Backend/3. ASP.NET/.NET.xlsx
+++ b/Backend/3. ASP.NET/.NET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janss\Desktop\Full stack\Backend-2024\3. ASP.NET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janss\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D79825-4EF6-4C4E-AE2B-6877C23C9D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80AD210-1F96-4E9A-8619-77B8EA1F0EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="1095" windowWidth="27000" windowHeight="13335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导航栏" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>2. LINQ</t>
-  </si>
-  <si>
-    <t>1. 异步编程</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>https://www.nuget.org/</t>
   </si>
@@ -61,22 +55,7 @@
     <t>包的下载</t>
   </si>
   <si>
-    <t>异步编程</t>
-  </si>
-  <si>
-    <t>想象，很多顾客来到餐厅，现在有两种点餐方式：</t>
-  </si>
-  <si>
-    <t>1. VIP服务，一位服务员接待一桌客户，协助顾客点完菜后，交给后厨，然后接待下一桌</t>
-  </si>
-  <si>
-    <t>2. 1对多，服务员拿着menu给顾客(然后接待其他桌客户)，顾客点完菜后call服务员，交给后厨，等待下一次点完菜call</t>
-  </si>
-  <si>
-    <t>问：这种方式可以加快单个客户的点餐速度吗？请问可以加快后厨做菜速度吗？</t>
-  </si>
-  <si>
-    <t>优点：可以同时服务多个客人</t>
+    <t>1. 包的下载</t>
   </si>
 </sst>
 </file>
@@ -156,15 +135,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>342165</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>47565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -200,15 +179,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>190176</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -244,15 +223,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>217993</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>152287</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -564,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2EBE1C-E390-409C-BB2C-BB5D71FEC225}">
-  <dimension ref="B2:J58"/>
+  <dimension ref="B3:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="U58" sqref="U58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,90 +554,61 @@
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="s">
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="s">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{0995FED0-B688-4775-ADC6-36192B145E68}"/>
+    <hyperlink ref="I9" r:id="rId1" xr:uid="{0995FED0-B688-4775-ADC6-36192B145E68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>